<commit_message>
add a str tag
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Monster.xlsx
+++ b/ConfigData/Xlsx/Monster.xlsx
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="Monster" sheetId="1" r:id="rId1"/>
+    <sheet name="~备注" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -51,6 +52,58 @@
   </si>
   <si>
     <t>老鼠</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>虫</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>兽</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>级别</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>鬼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>神</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸟</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Atk</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hp</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -802,14 +855,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <b val="0"/>
@@ -836,6 +882,44 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -947,6 +1031,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1029,15 +1120,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:C4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A3:C4"/>
-  <sortState ref="A4:C4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E4" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A3:E4"/>
+  <sortState ref="A4:E4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Id" dataDxfId="3"/>
-    <tableColumn id="2" name="Name" dataDxfId="2"/>
-    <tableColumn id="14" name="Url" dataDxfId="1"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Id" dataDxfId="4"/>
+    <tableColumn id="2" name="Name" dataDxfId="3"/>
+    <tableColumn id="3" name="Atk" dataDxfId="2"/>
+    <tableColumn id="4" name="Hp" dataDxfId="1"/>
+    <tableColumn id="14" name="Url" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1364,46 +1457,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9" style="4"/>
-    <col min="6" max="6" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="4"/>
+    <col min="2" max="7" width="9" style="4"/>
+    <col min="8" max="8" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -1411,24 +1516,36 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>41000001</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="10">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="0" priority="25">
+  <conditionalFormatting sqref="B4:E4">
+    <cfRule type="containsBlanks" dxfId="8" priority="25">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1438,4 +1555,95 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>